<commit_message>
18 de agosto (#12)
* 18 de jul,io

R terminado por Matilde

* 18 de agosto

camgio gdp nomaial
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -407,50 +407,55 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>gdp_nom</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>growth_pop</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>log_gdp_pc</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>gov_gdp</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>gov_con_gdp</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>pub_inv_gdp</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>priv_inv_gdp</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>tr_op</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>growth_gdp_pc</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>d_2008</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>d_2018</t>
         </is>
@@ -482,30 +487,33 @@
         <v>5618781.716412752</v>
       </c>
       <c r="I2">
+        <v>28404894621.76115</v>
+      </c>
+      <c r="J2">
         <v>0.003635164855745933</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>8.548596125140168</v>
       </c>
-      <c r="K2">
-        <v>0.1683227500207737</v>
-      </c>
       <c r="L2">
-        <v>0.1311961418392827</v>
+        <v>0.1717908075523179</v>
       </c>
       <c r="M2">
-        <v>0.03712660818149103</v>
+        <v>0.1338992569426131</v>
       </c>
       <c r="N2">
-        <v>0.1892428474754445</v>
+        <v>0.03789155060970478</v>
       </c>
       <c r="O2">
-        <v>0.8175925808262257</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
+        <v>0.1931419346897223</v>
+      </c>
+      <c r="P2">
+        <v>0.8344379455040191</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>0</v>
       </c>
     </row>
@@ -535,33 +543,36 @@
         <v>5639206.936322667</v>
       </c>
       <c r="I3">
+        <v>28595676297.39271</v>
+      </c>
+      <c r="J3">
         <v>0.003635168785833461</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>8.533790894958184</v>
       </c>
-      <c r="K3">
-        <v>0.1865399267654238</v>
-      </c>
       <c r="L3">
-        <v>0.1478516411448318</v>
+        <v>0.1870112602330128</v>
       </c>
       <c r="M3">
-        <v>0.03868828562059195</v>
+        <v>0.1482252202917625</v>
       </c>
       <c r="N3">
-        <v>0.1994679353144737</v>
+        <v>0.0387860399412504</v>
       </c>
       <c r="O3">
-        <v>0.9035754320871047</v>
+        <v>0.1999719341915765</v>
       </c>
       <c r="P3">
+        <v>0.9058585108307212</v>
+      </c>
+      <c r="Q3">
         <v>-0.001731890238497069</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>0</v>
       </c>
     </row>
@@ -591,33 +602,36 @@
         <v>5659706.46960453</v>
       </c>
       <c r="I4">
+        <v>29737151337.50516</v>
+      </c>
+      <c r="J4">
         <v>0.003635180179295043</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>8.565576525021916</v>
       </c>
-      <c r="K4">
-        <v>0.1692601648177922</v>
-      </c>
       <c r="L4">
-        <v>0.1369488701631498</v>
+        <v>0.1690565194328965</v>
       </c>
       <c r="M4">
-        <v>0.03231129465464233</v>
+        <v>0.1367841001157767</v>
       </c>
       <c r="N4">
-        <v>0.2161240443376031</v>
+        <v>0.03227241931711973</v>
       </c>
       <c r="O4">
-        <v>0.8871503109894318</v>
+        <v>0.2158640146711915</v>
       </c>
       <c r="P4">
+        <v>0.8860829360005424</v>
+      </c>
+      <c r="Q4">
         <v>0.003724678803942894</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
         <v>0</v>
       </c>
     </row>
@@ -647,33 +661,36 @@
         <v>5680280.417178485</v>
       </c>
       <c r="I5">
+        <v>32099987949.56785</v>
+      </c>
+      <c r="J5">
         <v>0.003635161590878802</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>8.62005212780468</v>
       </c>
-      <c r="K5">
-        <v>0.2434435768409516</v>
-      </c>
       <c r="L5">
-        <v>0.1878361980129923</v>
+        <v>0.2387285167735624</v>
       </c>
       <c r="M5">
-        <v>0.05560737882795933</v>
+        <v>0.1841981519082068</v>
       </c>
       <c r="N5">
-        <v>0.2039825973083534</v>
+        <v>0.05453036486535563</v>
       </c>
       <c r="O5">
-        <v>0.8831957113422567</v>
+        <v>0.2000318247659366</v>
       </c>
       <c r="P5">
+        <v>0.8660898140157485</v>
+      </c>
+      <c r="Q5">
         <v>0.006359829093071534</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>0</v>
       </c>
     </row>
@@ -703,33 +720,36 @@
         <v>5700929.082101099</v>
       </c>
       <c r="I6">
+        <v>32171235967.26353</v>
+      </c>
+      <c r="J6">
         <v>0.003635148866976427</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>8.570197614187531</v>
       </c>
-      <c r="K6">
-        <v>0.1722220003224474</v>
-      </c>
       <c r="L6">
-        <v>0.1442727517450762</v>
+        <v>0.1609000037596645</v>
       </c>
       <c r="M6">
-        <v>0.02794924857737128</v>
+        <v>0.1347881586251339</v>
       </c>
       <c r="N6">
-        <v>0.2199951016506926</v>
+        <v>0.02611184513453066</v>
       </c>
       <c r="O6">
-        <v>0.9295939473620598</v>
+        <v>0.2055324674921368</v>
       </c>
       <c r="P6">
+        <v>0.8684817813373266</v>
+      </c>
+      <c r="Q6">
         <v>-0.005783551291568045</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>0</v>
       </c>
     </row>
@@ -759,33 +779,36 @@
         <v>5721653.011171204</v>
       </c>
       <c r="I7">
+        <v>32873473464.92282</v>
+      </c>
+      <c r="J7">
         <v>0.003635184506183573</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>8.56629662730573</v>
       </c>
-      <c r="K7">
-        <v>0.1737480915831567</v>
-      </c>
       <c r="L7">
-        <v>0.1309212600350344</v>
+        <v>0.1588149274121401</v>
       </c>
       <c r="M7">
-        <v>0.04282683154812229</v>
+        <v>0.1196689426612702</v>
       </c>
       <c r="N7">
-        <v>0.2636926216395271</v>
+        <v>0.03914598475086987</v>
       </c>
       <c r="O7">
-        <v>1.012685090524654</v>
+        <v>0.2410289758190249</v>
       </c>
       <c r="P7">
+        <v>0.9256476297240687</v>
+      </c>
+      <c r="Q7">
         <v>-0.0004551805054463509</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
       <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
         <v>0</v>
       </c>
     </row>
@@ -794,7 +817,7 @@
         <v>39264</v>
       </c>
       <c r="B8">
-        <v>31258201751.44684</v>
+        <v>31258201751.44683</v>
       </c>
       <c r="C8">
         <v>4409774634.389752</v>
@@ -815,33 +838,36 @@
         <v>5742452.511547952</v>
       </c>
       <c r="I8">
-        <v>0.003635225753141372</v>
+        <v>34136537497.39998</v>
       </c>
       <c r="J8">
+        <v>0.003635225753141371</v>
+      </c>
+      <c r="K8">
         <v>8.602150690876083</v>
       </c>
-      <c r="K8">
-        <v>0.1807675478163191</v>
-      </c>
       <c r="L8">
-        <v>0.1410757621137191</v>
+        <v>0.1655255305312434</v>
       </c>
       <c r="M8">
-        <v>0.03969178570259997</v>
+        <v>0.1291804898117047</v>
       </c>
       <c r="N8">
-        <v>0.2294839755382622</v>
+        <v>0.03634504071953872</v>
       </c>
       <c r="O8">
-        <v>1.029746960782265</v>
+        <v>0.2101342705494206</v>
       </c>
       <c r="P8">
+        <v>0.9429204193753643</v>
+      </c>
+      <c r="Q8">
         <v>0.004185480042339984</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
       <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
         <v>0</v>
       </c>
     </row>
@@ -871,33 +897,36 @@
         <v>5763326.827382986</v>
       </c>
       <c r="I9">
+        <v>37768931535.66106</v>
+      </c>
+      <c r="J9">
         <v>0.003635087237213836</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>8.668017534597716</v>
       </c>
-      <c r="K9">
-        <v>0.2746726510593114</v>
-      </c>
       <c r="L9">
-        <v>0.1945239162313771</v>
+        <v>0.2436835162946204</v>
       </c>
       <c r="M9">
-        <v>0.08014873482793426</v>
+        <v>0.1725773269666602</v>
       </c>
       <c r="N9">
-        <v>0.2179095906845992</v>
+        <v>0.07110618932796016</v>
       </c>
       <c r="O9">
-        <v>1.099490898549681</v>
+        <v>0.1933245814155638</v>
       </c>
       <c r="P9">
+        <v>0.9754440686366808</v>
+      </c>
+      <c r="Q9">
         <v>0.007657020446234952</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
       <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
         <v>0</v>
       </c>
     </row>
@@ -924,36 +953,39 @@
         <v>23786609961.86752</v>
       </c>
       <c r="H10">
-        <v>5784277.08504153</v>
+        <v>5784277.085041529</v>
       </c>
       <c r="I10">
-        <v>0.003635097971366927</v>
+        <v>38502079141.78066</v>
       </c>
       <c r="J10">
+        <v>0.003635097971366926</v>
+      </c>
+      <c r="K10">
         <v>8.612114267510332</v>
       </c>
-      <c r="K10">
-        <v>0.180918377295483</v>
-      </c>
       <c r="L10">
-        <v>0.1396038530853629</v>
+        <v>0.1494312034824594</v>
       </c>
       <c r="M10">
-        <v>0.04131452421012002</v>
+        <v>0.1153070909057677</v>
       </c>
       <c r="N10">
-        <v>0.2846727585656139</v>
+        <v>0.03412411257669167</v>
       </c>
       <c r="O10">
-        <v>1.203061300054715</v>
+        <v>0.2351280922758607</v>
       </c>
       <c r="P10">
+        <v>0.9936795842289301</v>
+      </c>
+      <c r="Q10">
         <v>-0.006449371712072605</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
       <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
         <v>0</v>
       </c>
     </row>
@@ -962,7 +994,7 @@
         <v>39539</v>
       </c>
       <c r="B11">
-        <v>32304815368.96808</v>
+        <v>32304815368.96807</v>
       </c>
       <c r="C11">
         <v>5568980818.152805</v>
@@ -983,33 +1015,36 @@
         <v>5805304.824068742</v>
       </c>
       <c r="I11">
+        <v>40923372072.55576</v>
+      </c>
+      <c r="J11">
         <v>0.00363532706301216</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>8.624199456352249</v>
       </c>
-      <c r="K11">
-        <v>0.2407000815366384</v>
-      </c>
       <c r="L11">
-        <v>0.1723885666748727</v>
+        <v>0.1900080882765595</v>
       </c>
       <c r="M11">
-        <v>0.06831151486176565</v>
+        <v>0.136083136264509</v>
       </c>
       <c r="N11">
-        <v>0.3000930010721871</v>
+        <v>0.05392495201205053</v>
       </c>
       <c r="O11">
-        <v>1.297671489009045</v>
+        <v>0.2368927217426905</v>
       </c>
       <c r="P11">
-        <v>0.001403277809203019</v>
+        <v>1.024378875418343</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>0.001403277809203018</v>
       </c>
       <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
         <v>0</v>
       </c>
     </row>
@@ -1039,33 +1074,36 @@
         <v>5826409.375474685</v>
       </c>
       <c r="I12">
+        <v>42563052253.84702</v>
+      </c>
+      <c r="J12">
         <v>0.003635390740972563</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>8.626000084807492</v>
       </c>
-      <c r="K12">
-        <v>0.2493854837909823</v>
-      </c>
       <c r="L12">
-        <v>0.1831580623403763</v>
+        <v>0.1903108897823829</v>
       </c>
       <c r="M12">
-        <v>0.06622742145060606</v>
+        <v>0.1397714625765021</v>
       </c>
       <c r="N12">
-        <v>0.2695715079441047</v>
+        <v>0.05053942720588076</v>
       </c>
       <c r="O12">
-        <v>1.288216921741898</v>
+        <v>0.2057152355339951</v>
       </c>
       <c r="P12">
+        <v>0.9830632676876273</v>
+      </c>
+      <c r="Q12">
         <v>0.0002087878955439049</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
       <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
         <v>0</v>
       </c>
     </row>
@@ -1086,7 +1124,7 @@
         <v>8360640164.096471</v>
       </c>
       <c r="F13">
-        <v>12432352308.93016</v>
+        <v>12432352308.93015</v>
       </c>
       <c r="G13">
         <v>24870902079.54176</v>
@@ -1095,33 +1133,36 @@
         <v>5847585.653632261</v>
       </c>
       <c r="I13">
+        <v>42613869181.54015</v>
+      </c>
+      <c r="J13">
         <v>0.003634533173503695</v>
       </c>
-      <c r="J13">
-        <v>8.625236837508505</v>
-      </c>
       <c r="K13">
-        <v>0.2959797229765067</v>
+        <v>8.625236837508504</v>
       </c>
       <c r="L13">
-        <v>0.2093706735050749</v>
+        <v>0.2262457066777378</v>
       </c>
       <c r="M13">
-        <v>0.08660904947143189</v>
+        <v>0.1600420985207473</v>
       </c>
       <c r="N13">
-        <v>0.256667083960424</v>
+        <v>0.06620360815699056</v>
       </c>
       <c r="O13">
-        <v>1.14518952355339</v>
+        <v>0.1961952839456833</v>
       </c>
       <c r="P13">
-        <v>-8.848218078871817e-005</v>
+        <v>0.8753782537219423</v>
       </c>
       <c r="Q13">
+        <v>-8.848218078871817e-05</v>
+      </c>
+      <c r="R13">
         <v>1</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>0</v>
       </c>
     </row>
@@ -1151,33 +1192,36 @@
         <v>5868842.451454693</v>
       </c>
       <c r="I14">
+        <v>40836535457.64165</v>
+      </c>
+      <c r="J14">
         <v>0.003635140907979287</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>8.544161659293268</v>
       </c>
-      <c r="K14">
-        <v>0.2585983981491451</v>
-      </c>
       <c r="L14">
-        <v>0.1948866986211504</v>
+        <v>0.1909025162681806</v>
       </c>
       <c r="M14">
-        <v>0.06371169952799473</v>
+        <v>0.1438692637706084</v>
       </c>
       <c r="N14">
-        <v>0.2159914258952123</v>
+        <v>0.0470332524975722</v>
       </c>
       <c r="O14">
-        <v>1.12622778286167</v>
+        <v>0.1594491960927276</v>
       </c>
       <c r="P14">
+        <v>0.8314039034202645</v>
+      </c>
+      <c r="Q14">
         <v>-0.00939976255059638</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>1</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>0</v>
       </c>
     </row>
@@ -1207,33 +1251,36 @@
         <v>5890182.991258112</v>
       </c>
       <c r="I15">
+        <v>40679474743.56019</v>
+      </c>
+      <c r="J15">
         <v>0.003636243429593097</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>8.545893952453072</v>
       </c>
-      <c r="K15">
-        <v>0.2584565040066593</v>
-      </c>
       <c r="L15">
-        <v>0.1790618551374628</v>
+        <v>0.1925641791508088</v>
       </c>
       <c r="M15">
-        <v>0.07939464886919652</v>
+        <v>0.133410839414891</v>
       </c>
       <c r="N15">
-        <v>0.2048851331088027</v>
+        <v>0.05915333973591783</v>
       </c>
       <c r="O15">
-        <v>1.180607555525651</v>
+        <v>0.1526505886510183</v>
       </c>
       <c r="P15">
+        <v>0.8796169618667535</v>
+      </c>
+      <c r="Q15">
         <v>0.0002027458314672881</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>1</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>0</v>
       </c>
     </row>
@@ -1263,33 +1310,36 @@
         <v>5911597.608266522</v>
       </c>
       <c r="I16">
+        <v>42491795704.36271</v>
+      </c>
+      <c r="J16">
         <v>0.003635645452814174</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>8.581176323267574</v>
       </c>
-      <c r="K16">
-        <v>0.2526317743775057</v>
-      </c>
       <c r="L16">
-        <v>0.1865612625900797</v>
+        <v>0.1873463678962472</v>
       </c>
       <c r="M16">
-        <v>0.06607051178742601</v>
+        <v>0.1383498770988386</v>
       </c>
       <c r="N16">
-        <v>0.1835672786566354</v>
+        <v>0.04899649079740855</v>
       </c>
       <c r="O16">
-        <v>1.188400711206043</v>
+        <v>0.1361296020884896</v>
       </c>
       <c r="P16">
+        <v>0.8812927724486311</v>
+      </c>
+      <c r="Q16">
         <v>0.004128575782803123</v>
       </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
       <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
         <v>0</v>
       </c>
     </row>
@@ -1319,33 +1369,36 @@
         <v>5933063.22750698</v>
       </c>
       <c r="I17">
+        <v>44783504022.36033</v>
+      </c>
+      <c r="J17">
         <v>0.003631102903628222</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>8.621960336949027</v>
       </c>
-      <c r="K17">
-        <v>0.3254728682300608</v>
-      </c>
       <c r="L17">
-        <v>0.2213008674053631</v>
+        <v>0.2394117680437255</v>
       </c>
       <c r="M17">
-        <v>0.1041720008246977</v>
+        <v>0.1627847882474728</v>
       </c>
       <c r="N17">
-        <v>0.1804443082283408</v>
+        <v>0.07662697979625274</v>
       </c>
       <c r="O17">
-        <v>1.203813967053018</v>
+        <v>0.1327314657633389</v>
       </c>
       <c r="P17">
+        <v>0.8855030891366787</v>
+      </c>
+      <c r="Q17">
         <v>0.00475272994576148</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
       <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
         <v>0</v>
       </c>
     </row>
@@ -1363,7 +1416,7 @@
         <v>1737017831.342906</v>
       </c>
       <c r="E18">
-        <v>6291616565.443934</v>
+        <v>6291616565.443933</v>
       </c>
       <c r="F18">
         <v>18223356565.4394</v>
@@ -1375,33 +1428,36 @@
         <v>5954645.171263196</v>
       </c>
       <c r="I18">
+        <v>44245470140.01509</v>
+      </c>
+      <c r="J18">
         <v>0.003637571845881654</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>8.565704969950156</v>
       </c>
-      <c r="K18">
-        <v>0.2740813994786094</v>
-      </c>
       <c r="L18">
-        <v>0.218502494367039</v>
+        <v>0.1935998598934056</v>
       </c>
       <c r="M18">
-        <v>0.05557890511157047</v>
+        <v>0.1543412007392345</v>
       </c>
       <c r="N18">
-        <v>0.2013112092343067</v>
+        <v>0.03925865915417107</v>
       </c>
       <c r="O18">
-        <v>1.320925842609147</v>
+        <v>0.1421979819749699</v>
       </c>
       <c r="P18">
+        <v>0.9330478410617864</v>
+      </c>
+      <c r="Q18">
         <v>-0.006524660842823771</v>
       </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
       <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
         <v>0</v>
       </c>
     </row>
@@ -1431,33 +1487,36 @@
         <v>5976323.971142774</v>
       </c>
       <c r="I19">
+        <v>43898832106.09261</v>
+      </c>
+      <c r="J19">
         <v>0.003640653516048339</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>8.565703128152842</v>
       </c>
-      <c r="K19">
-        <v>0.245273001877905</v>
-      </c>
       <c r="L19">
-        <v>0.1697348549534433</v>
+        <v>0.1752542321623349</v>
       </c>
       <c r="M19">
-        <v>0.07553814692446169</v>
+        <v>0.1212801712715968</v>
       </c>
       <c r="N19">
-        <v>0.2165129141679142</v>
+        <v>0.05397406089073813</v>
       </c>
       <c r="O19">
-        <v>1.496089717682644</v>
+        <v>0.1547043671142247</v>
       </c>
       <c r="P19">
-        <v>-2.150199336359293e-007</v>
+        <v>1.068996802383311</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>-2.150199336359293e-07</v>
       </c>
       <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
         <v>0</v>
       </c>
     </row>
@@ -1487,33 +1546,36 @@
         <v>5998037.471401172</v>
       </c>
       <c r="I20">
+        <v>47098605699.23959</v>
+      </c>
+      <c r="J20">
         <v>0.003633253545698482</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>8.613491336783337</v>
       </c>
-      <c r="K20">
-        <v>0.2393096982963532</v>
-      </c>
       <c r="L20">
-        <v>0.1828392658404943</v>
+        <v>0.1677850187570495</v>
       </c>
       <c r="M20">
-        <v>0.05647043245585888</v>
+        <v>0.1281924212305941</v>
       </c>
       <c r="N20">
-        <v>0.240987895832623</v>
+        <v>0.03959259752645539</v>
       </c>
       <c r="O20">
-        <v>1.471959651147033</v>
+        <v>0.1689616380378626</v>
       </c>
       <c r="P20">
+        <v>1.032021599774373</v>
+      </c>
+      <c r="Q20">
         <v>0.005579017614260939</v>
       </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
       <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
         <v>0</v>
       </c>
     </row>
@@ -1534,7 +1596,7 @@
         <v>8848696152.767782</v>
       </c>
       <c r="F21">
-        <v>19185768703.31373</v>
+        <v>19185768703.31372</v>
       </c>
       <c r="G21">
         <v>31730224162.81681</v>
@@ -1543,33 +1605,36 @@
         <v>6019707.977158715</v>
       </c>
       <c r="I21">
+        <v>51809733906.81725</v>
+      </c>
+      <c r="J21">
         <v>0.003612932706884413</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>8.661596343339069</v>
       </c>
-      <c r="K21">
-        <v>0.3428927024713842</v>
-      </c>
       <c r="L21">
-        <v>0.2351884184714119</v>
+        <v>0.2301472557154489</v>
       </c>
       <c r="M21">
-        <v>0.1077042839999723</v>
+        <v>0.1578568709602948</v>
       </c>
       <c r="N21">
-        <v>0.2544604919580081</v>
+        <v>0.07229038475515413</v>
       </c>
       <c r="O21">
-        <v>1.464182786883633</v>
+        <v>0.1707921559427938</v>
       </c>
       <c r="P21">
+        <v>0.9827495535434683</v>
+      </c>
+      <c r="Q21">
         <v>0.005584844132866529</v>
       </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
       <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
         <v>0</v>
       </c>
     </row>
@@ -1599,33 +1664,36 @@
         <v>6041760.861990004</v>
       </c>
       <c r="I22">
+        <v>49878976144.41065</v>
+      </c>
+      <c r="J22">
         <v>0.003663447614895382</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>8.605613255744078</v>
       </c>
-      <c r="K22">
-        <v>0.288125666335863</v>
-      </c>
       <c r="L22">
-        <v>0.2046787525246525</v>
+        <v>0.1906330949645199</v>
       </c>
       <c r="M22">
-        <v>0.0834469138112105</v>
+        <v>0.1354219655730647</v>
       </c>
       <c r="N22">
-        <v>0.2802879978647859</v>
+        <v>0.05521112939145526</v>
       </c>
       <c r="O22">
-        <v>1.765975413706243</v>
+        <v>0.1854474444914184</v>
       </c>
       <c r="P22">
+        <v>1.168425440979766</v>
+      </c>
+      <c r="Q22">
         <v>-0.006463368341800169</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
       <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
         <v>0</v>
       </c>
     </row>
@@ -1655,33 +1723,36 @@
         <v>6063831.294772142</v>
       </c>
       <c r="I23">
+        <v>53615947580.80576</v>
+      </c>
+      <c r="J23">
         <v>0.003652980196715079</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>8.625660835667087</v>
       </c>
-      <c r="K23">
-        <v>0.2899009616024695</v>
-      </c>
       <c r="L23">
-        <v>0.2061069585016653</v>
+        <v>0.1827173061802906</v>
       </c>
       <c r="M23">
-        <v>0.08379400310080422</v>
+        <v>0.1299040473486875</v>
       </c>
       <c r="N23">
-        <v>0.2974103169298947</v>
+        <v>0.05281325883160315</v>
       </c>
       <c r="O23">
-        <v>1.822372414349857</v>
+        <v>0.1874502645292155</v>
       </c>
       <c r="P23">
+        <v>1.148595632683275</v>
+      </c>
+      <c r="Q23">
         <v>0.002329593409235331</v>
       </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
       <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
         <v>0</v>
       </c>
     </row>
@@ -1711,33 +1782,36 @@
         <v>6085683.242637239</v>
       </c>
       <c r="I24">
+        <v>55971206003.80614</v>
+      </c>
+      <c r="J24">
         <v>0.003603653664299054</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>8.669335269580563</v>
       </c>
-      <c r="K24">
-        <v>0.2849631091444164</v>
-      </c>
       <c r="L24">
-        <v>0.2165225407641633</v>
+        <v>0.1803756001143096</v>
       </c>
       <c r="M24">
-        <v>0.06844056838025302</v>
+        <v>0.137054172892317</v>
       </c>
       <c r="N24">
-        <v>0.3122485059297431</v>
+        <v>0.04332142722199266</v>
       </c>
       <c r="O24">
-        <v>1.750976854703686</v>
+        <v>0.1976466771820999</v>
       </c>
       <c r="P24">
+        <v>1.108331186804192</v>
+      </c>
+      <c r="Q24">
         <v>0.00506331453850839</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
       <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
         <v>0</v>
       </c>
     </row>
@@ -1746,7 +1820,7 @@
         <v>40817</v>
       </c>
       <c r="B25">
-        <v>36431348061.03198</v>
+        <v>36431348061.03197</v>
       </c>
       <c r="C25">
         <v>8415184478.565527</v>
@@ -1767,33 +1841,36 @@
         <v>6107175.741915314</v>
       </c>
       <c r="I25">
+        <v>59716080079.41579</v>
+      </c>
+      <c r="J25">
         <v>0.003531649351628137</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>8.693720462509724</v>
       </c>
-      <c r="K25">
-        <v>0.3297822018064353</v>
-      </c>
       <c r="L25">
-        <v>0.2309874579570294</v>
+        <v>0.2011922109148138</v>
       </c>
       <c r="M25">
-        <v>0.09879474384940593</v>
+        <v>0.1409199074583305</v>
       </c>
       <c r="N25">
-        <v>0.3290208672035519</v>
+        <v>0.06027230345648329</v>
       </c>
       <c r="O25">
-        <v>1.734998755222961</v>
+        <v>0.2007277389355468</v>
       </c>
       <c r="P25">
+        <v>1.05848112355876</v>
+      </c>
+      <c r="Q25">
         <v>0.00281280999879252</v>
       </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
       <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
         <v>0</v>
       </c>
     </row>
@@ -1823,33 +1900,36 @@
         <v>6130783.07400402</v>
       </c>
       <c r="I26">
+        <v>60018153182.96165</v>
+      </c>
+      <c r="J26">
         <v>0.003865507246939256</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>8.679381767370222</v>
       </c>
-      <c r="K26">
-        <v>0.3452537497866674</v>
-      </c>
       <c r="L26">
-        <v>0.2585823297595835</v>
+        <v>0.2073859517625361</v>
       </c>
       <c r="M26">
-        <v>0.08667142002708392</v>
+        <v>0.1553244319556296</v>
       </c>
       <c r="N26">
-        <v>0.3614568878063224</v>
+        <v>0.05206151980690652</v>
       </c>
       <c r="O26">
-        <v>1.916091226644959</v>
+        <v>0.2171188024609636</v>
       </c>
       <c r="P26">
+        <v>1.150951736069907</v>
+      </c>
+      <c r="Q26">
         <v>-0.001649316331406747</v>
       </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
       <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
         <v>0</v>
       </c>
     </row>
@@ -1879,33 +1959,36 @@
         <v>6152922.009282879</v>
       </c>
       <c r="I27">
+        <v>58823460864.84393</v>
+      </c>
+      <c r="J27">
         <v>0.00361111052399387</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>8.656118642286431</v>
       </c>
-      <c r="K27">
-        <v>0.2612085452003666</v>
-      </c>
       <c r="L27">
-        <v>0.1735027811648765</v>
+        <v>0.1569722123291996</v>
       </c>
       <c r="M27">
-        <v>0.08770576403549013</v>
+        <v>0.104265790324081</v>
       </c>
       <c r="N27">
-        <v>0.3906892785359042</v>
+        <v>0.05270642200511867</v>
       </c>
       <c r="O27">
-        <v>2.033683306417379</v>
+        <v>0.2347831321446129</v>
       </c>
       <c r="P27">
+        <v>1.222133707534042</v>
+      </c>
+      <c r="Q27">
         <v>-0.002680274437431351</v>
       </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
       <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
         <v>0</v>
       </c>
     </row>
@@ -1935,33 +2018,36 @@
         <v>6173881</v>
       </c>
       <c r="I28">
+        <v>61911265449.46594</v>
+      </c>
+      <c r="J28">
         <v>0.003406347534634951</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>8.691893710688811</v>
       </c>
-      <c r="K28">
-        <v>0.2831373784920303</v>
-      </c>
       <c r="L28">
-        <v>0.2172634761527185</v>
+        <v>0.168123048353181</v>
       </c>
       <c r="M28">
-        <v>0.06587390233931184</v>
+        <v>0.1290080387871919</v>
       </c>
       <c r="N28">
-        <v>0.381731476414839</v>
+        <v>0.03911500956598912</v>
       </c>
       <c r="O28">
-        <v>1.912839131521154</v>
+        <v>0.2266668562414115</v>
       </c>
       <c r="P28">
+        <v>1.13581734602957</v>
+      </c>
+      <c r="Q28">
         <v>0.004132922604319855</v>
       </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
       <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
         <v>0</v>
       </c>
     </row>
@@ -1991,33 +2077,36 @@
         <v>6189844</v>
       </c>
       <c r="I29">
+        <v>67240991467.8511</v>
+      </c>
+      <c r="J29">
         <v>0.003243632100944471</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>8.761098374526338</v>
       </c>
-      <c r="K29">
-        <v>0.3864732189890803</v>
-      </c>
       <c r="L29">
-        <v>0.2584134296244087</v>
+        <v>0.2270187245011112</v>
       </c>
       <c r="M29">
-        <v>0.1280597893646716</v>
+        <v>0.1517949609567862</v>
       </c>
       <c r="N29">
-        <v>0.3802447244288822</v>
+        <v>0.07522376354432504</v>
       </c>
       <c r="O29">
-        <v>1.882231414204043</v>
+        <v>0.223360036599484</v>
       </c>
       <c r="P29">
+        <v>1.105643946005475</v>
+      </c>
+      <c r="Q29">
         <v>0.007961977693356159</v>
       </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
       <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
         <v>0</v>
       </c>
     </row>
@@ -2038,7 +2127,7 @@
         <v>14140736489.60429</v>
       </c>
       <c r="F30">
-        <v>29165099526.34609</v>
+        <v>29165099526.34608</v>
       </c>
       <c r="G30">
         <v>39516871463.70847</v>
@@ -2047,33 +2136,36 @@
         <v>6222037</v>
       </c>
       <c r="I30">
+        <v>65473325256.02543</v>
+      </c>
+      <c r="J30">
         <v>0.005200938828183732</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>8.699035229473841</v>
       </c>
-      <c r="K30">
-        <v>0.3293066792586696</v>
-      </c>
       <c r="L30">
-        <v>0.2213130749675731</v>
+        <v>0.1876772920544502</v>
       </c>
       <c r="M30">
-        <v>0.1079936042910965</v>
+        <v>0.1261299609824544</v>
       </c>
       <c r="N30">
-        <v>0.378962679041838</v>
+        <v>0.06154733107199572</v>
       </c>
       <c r="O30">
-        <v>1.840632823290325</v>
+        <v>0.2159770629383596</v>
       </c>
       <c r="P30">
+        <v>1.049006915739839</v>
+      </c>
+      <c r="Q30">
         <v>-0.007083945688014515</v>
       </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
       <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
         <v>0</v>
       </c>
     </row>
@@ -2103,33 +2195,36 @@
         <v>6238174</v>
       </c>
       <c r="I31">
+        <v>66888903715.75397</v>
+      </c>
+      <c r="J31">
         <v>0.002593523632212325</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>8.712088944654084</v>
       </c>
-      <c r="K31">
-        <v>0.3542417852904302</v>
-      </c>
       <c r="L31">
-        <v>0.2387773631068416</v>
+        <v>0.200731416197046</v>
       </c>
       <c r="M31">
-        <v>0.1154644221835886</v>
+        <v>0.1353034007914577</v>
       </c>
       <c r="N31">
-        <v>0.4118834859520127</v>
+        <v>0.06542801540558825</v>
       </c>
       <c r="O31">
-        <v>1.971338769668048</v>
+        <v>0.2333941360857215</v>
       </c>
       <c r="P31">
+        <v>1.117060830966571</v>
+      </c>
+      <c r="Q31">
         <v>0.001500593437765874</v>
       </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
       <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
         <v>0</v>
       </c>
     </row>
@@ -2141,7 +2236,7 @@
         <v>38983539408.59612</v>
       </c>
       <c r="C32">
-        <v>9014004571.717156</v>
+        <v>9014004571.717155</v>
       </c>
       <c r="D32">
         <v>3663934920.260924</v>
@@ -2159,33 +2254,36 @@
         <v>6254314</v>
       </c>
       <c r="I32">
+        <v>68626247533.24363</v>
+      </c>
+      <c r="J32">
         <v>0.002587295577199278</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>8.737623303928176</v>
       </c>
-      <c r="K32">
-        <v>0.3252126329294388</v>
-      </c>
       <c r="L32">
-        <v>0.2312259150519696</v>
+        <v>0.1847389293118014</v>
       </c>
       <c r="M32">
-        <v>0.09398671787746915</v>
+        <v>0.1313492270920194</v>
       </c>
       <c r="N32">
-        <v>0.41712316002587</v>
+        <v>0.05338970221978197</v>
       </c>
       <c r="O32">
-        <v>2.020816354801347</v>
+        <v>0.2369492392721837</v>
       </c>
       <c r="P32">
+        <v>1.14793649422216</v>
+      </c>
+      <c r="Q32">
         <v>0.002930911224197308</v>
       </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
       <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
         <v>0</v>
       </c>
     </row>
@@ -2215,33 +2313,36 @@
         <v>6270530</v>
       </c>
       <c r="I33">
+        <v>70541349947.52602</v>
+      </c>
+      <c r="J33">
         <v>0.002592770366182551</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>8.779014013148084</v>
       </c>
-      <c r="K33">
-        <v>0.376314013956005</v>
-      </c>
       <c r="L33">
-        <v>0.2711540951894462</v>
+        <v>0.217314256189573</v>
       </c>
       <c r="M33">
-        <v>0.1051599187665588</v>
+        <v>0.1565863835082692</v>
       </c>
       <c r="N33">
-        <v>0.3583177041067836</v>
+        <v>0.06072787268130379</v>
       </c>
       <c r="O33">
-        <v>1.943615535932722</v>
+        <v>0.206921726164109</v>
       </c>
       <c r="P33">
+        <v>1.1224013691903</v>
+      </c>
+      <c r="Q33">
         <v>0.004737067252750471</v>
       </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
       <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
         <v>0</v>
       </c>
     </row>
@@ -2271,33 +2372,36 @@
         <v>6303139</v>
       </c>
       <c r="I34">
+        <v>73750654936.6973</v>
+      </c>
+      <c r="J34">
         <v>0.005200357864486804</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>8.739832045976259</v>
       </c>
-      <c r="K34">
-        <v>0.3838910115206692</v>
-      </c>
       <c r="L34">
-        <v>0.2682596594359126</v>
+        <v>0.2049555943467155</v>
       </c>
       <c r="M34">
-        <v>0.1156313520847566</v>
+        <v>0.1432211650935586</v>
       </c>
       <c r="N34">
-        <v>0.3867579195029171</v>
+        <v>0.06173442925315694</v>
       </c>
       <c r="O34">
-        <v>1.990414268135063</v>
+        <v>0.2064862080151924</v>
       </c>
       <c r="P34">
+        <v>1.062662388748949</v>
+      </c>
+      <c r="Q34">
         <v>-0.004463139837018515</v>
       </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
       <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
         <v>0</v>
       </c>
     </row>
@@ -2327,33 +2431,36 @@
         <v>6319442</v>
       </c>
       <c r="I35">
+        <v>73592368589.71155</v>
+      </c>
+      <c r="J35">
         <v>0.002586489049344998</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>8.738159627349759</v>
       </c>
-      <c r="K35">
-        <v>0.385282691092569</v>
-      </c>
       <c r="L35">
-        <v>0.2705137804593365</v>
+        <v>0.2063288502086486</v>
       </c>
       <c r="M35">
-        <v>0.1147689106332325</v>
+        <v>0.1448671289371769</v>
       </c>
       <c r="N35">
-        <v>0.3858019115737853</v>
+        <v>0.06146172127147168</v>
       </c>
       <c r="O35">
-        <v>2.055146780410234</v>
+        <v>0.2066069062110876</v>
       </c>
       <c r="P35">
+        <v>1.100584277506953</v>
+      </c>
+      <c r="Q35">
         <v>-0.0001913559228257089</v>
       </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
       <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
         <v>0</v>
       </c>
     </row>
@@ -2383,33 +2490,36 @@
         <v>6335896</v>
       </c>
       <c r="I36">
+        <v>78192046594.51315</v>
+      </c>
+      <c r="J36">
         <v>0.002603710897259637</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>8.760437197366034</v>
       </c>
-      <c r="K36">
-        <v>0.3514547798127548</v>
-      </c>
       <c r="L36">
-        <v>0.2595983113732979</v>
+        <v>0.1816035974988915</v>
       </c>
       <c r="M36">
-        <v>0.09185646843945683</v>
+        <v>0.1341395535298888</v>
       </c>
       <c r="N36">
-        <v>0.3859040659150006</v>
+        <v>0.04746404396900269</v>
       </c>
       <c r="O36">
-        <v>2.050752319154029</v>
+        <v>0.1994042212114769</v>
       </c>
       <c r="P36">
-        <v>0.002549457891172891</v>
+        <v>1.059664059586794</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>0.00254945789117289</v>
       </c>
       <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
         <v>0</v>
       </c>
     </row>
@@ -2439,33 +2549,36 @@
         <v>6352515</v>
       </c>
       <c r="I37">
+        <v>82868053243.88741</v>
+      </c>
+      <c r="J37">
         <v>0.002622991286473031</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <v>8.823877315489048</v>
       </c>
-      <c r="K37">
-        <v>0.4197877136565241</v>
-      </c>
       <c r="L37">
-        <v>0.2855778200998436</v>
+        <v>0.2186500159739874</v>
       </c>
       <c r="M37">
-        <v>0.1342098935566804</v>
+        <v>0.1487456466573432</v>
       </c>
       <c r="N37">
-        <v>0.4562267328750678</v>
+        <v>0.06990436931664414</v>
       </c>
       <c r="O37">
-        <v>2.011852012380519</v>
+        <v>0.2376295903517407</v>
       </c>
       <c r="P37">
+        <v>1.047890303440906</v>
+      </c>
+      <c r="Q37">
         <v>0.007241661197238791</v>
       </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
       <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
         <v>0</v>
       </c>
     </row>
@@ -2486,7 +2599,7 @@
         <v>18351176273.44638</v>
       </c>
       <c r="F38">
-        <v>35047178572.14871</v>
+        <v>35047178572.1487</v>
       </c>
       <c r="G38">
         <v>47102950469.85974</v>
@@ -2495,33 +2608,36 @@
         <v>6385245</v>
       </c>
       <c r="I38">
+        <v>82858815507.12787</v>
+      </c>
+      <c r="J38">
         <v>0.005152290077237165</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>8.772064316009129</v>
       </c>
-      <c r="K38">
-        <v>0.457281801057404</v>
-      </c>
       <c r="L38">
-        <v>0.3306360994818703</v>
+        <v>0.227343158826692</v>
       </c>
       <c r="M38">
-        <v>0.1266457015755337</v>
+        <v>0.1643797218794385</v>
       </c>
       <c r="N38">
-        <v>0.4454789771972425</v>
+        <v>0.06296343694725354</v>
       </c>
       <c r="O38">
-        <v>1.994213063890023</v>
+        <v>0.2214752426899916</v>
       </c>
       <c r="P38">
+        <v>0.9914470601494605</v>
+      </c>
+      <c r="Q38">
         <v>-0.005871908417059313</v>
       </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
       <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
         <v>0</v>
       </c>
     </row>
@@ -2551,33 +2667,36 @@
         <v>6401820</v>
       </c>
       <c r="I39">
+        <v>83006884948.08031</v>
+      </c>
+      <c r="J39">
         <v>0.002595828351144025</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>8.754293342367847</v>
       </c>
-      <c r="K39">
-        <v>0.3941781481756642</v>
-      </c>
       <c r="L39">
-        <v>0.2330517055040285</v>
+        <v>0.1926740291054423</v>
       </c>
       <c r="M39">
-        <v>0.1611264426716357</v>
+        <v>0.1139155260056305</v>
       </c>
       <c r="N39">
-        <v>0.4371349835287824</v>
+        <v>0.07875850309981181</v>
       </c>
       <c r="O39">
-        <v>2.076924685500654</v>
+        <v>0.2136713030116963</v>
       </c>
       <c r="P39">
+        <v>1.015199470483154</v>
+      </c>
+      <c r="Q39">
         <v>-0.002025859934570939</v>
       </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
       <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
         <v>0</v>
       </c>
     </row>
@@ -2586,7 +2705,7 @@
         <v>42186</v>
       </c>
       <c r="B40">
-        <v>42971945220.09905</v>
+        <v>42971945220.09904</v>
       </c>
       <c r="C40">
         <v>11565942716.45308</v>
@@ -2598,7 +2717,7 @@
         <v>19085430365.47343</v>
       </c>
       <c r="F40">
-        <v>35845089833.30953</v>
+        <v>35845089833.30952</v>
       </c>
       <c r="G40">
         <v>50503621673.79926</v>
@@ -2607,33 +2726,36 @@
         <v>6418495</v>
       </c>
       <c r="I40">
+        <v>88367745971.51514</v>
+      </c>
+      <c r="J40">
         <v>0.002604728030466408</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>8.809119078460013</v>
       </c>
-      <c r="K40">
-        <v>0.3977253660713196</v>
-      </c>
       <c r="L40">
-        <v>0.2691510160225049</v>
+        <v>0.1934080410851465</v>
       </c>
       <c r="M40">
-        <v>0.1285743500488147</v>
+        <v>0.1308842110806051</v>
       </c>
       <c r="N40">
-        <v>0.4441369890918204</v>
+        <v>0.06252383000454134</v>
       </c>
       <c r="O40">
-        <v>2.009420589755414</v>
+        <v>0.215977336025132</v>
       </c>
       <c r="P40">
+        <v>0.9771519071556133</v>
+      </c>
+      <c r="Q40">
         <v>0.006262725493424881</v>
       </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
       <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
         <v>0</v>
       </c>
     </row>
@@ -2663,33 +2785,36 @@
         <v>6435097</v>
       </c>
       <c r="I41">
+        <v>93473846296.43387</v>
+      </c>
+      <c r="J41">
         <v>0.002586587665800222</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>8.861316552801046</v>
       </c>
-      <c r="K41">
-        <v>0.5066688121287986</v>
-      </c>
       <c r="L41">
-        <v>0.3132479348834768</v>
+        <v>0.2460424469894418</v>
       </c>
       <c r="M41">
-        <v>0.1934208772453218</v>
+        <v>0.1521157145814763</v>
       </c>
       <c r="N41">
-        <v>0.4520498983863978</v>
+        <v>0.09392673240796551</v>
       </c>
       <c r="O41">
-        <v>1.953242132429856</v>
+        <v>0.2195190635338417</v>
       </c>
       <c r="P41">
-        <v>0.005925390935929809</v>
+        <v>0.9485100766449985</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>0.005925390935929808</v>
       </c>
       <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
         <v>0</v>
       </c>
     </row>
@@ -2704,7 +2829,7 @@
         <v>13088767500.29381</v>
       </c>
       <c r="D42">
-        <v>7158657013.794169</v>
+        <v>7158657013.794168</v>
       </c>
       <c r="E42">
         <v>18385622915.30467</v>
@@ -2719,33 +2844,36 @@
         <v>6465879</v>
       </c>
       <c r="I42">
+        <v>91564338112.25935</v>
+      </c>
+      <c r="J42">
         <v>0.00478345547860437</v>
       </c>
-      <c r="J42">
-        <v>8.798839853675752</v>
-      </c>
       <c r="K42">
-        <v>0.4725574559353072</v>
+        <v>8.798839853675751</v>
       </c>
       <c r="L42">
-        <v>0.3054805645510109</v>
+        <v>0.2211278422529993</v>
       </c>
       <c r="M42">
-        <v>0.1670768913842964</v>
+        <v>0.1429461269544347</v>
       </c>
       <c r="N42">
-        <v>0.4291046095564918</v>
+        <v>0.0781817152985646</v>
       </c>
       <c r="O42">
-        <v>2.00771245429546</v>
+        <v>0.2007945811038747</v>
       </c>
       <c r="P42">
+        <v>0.9394860186982352</v>
+      </c>
+      <c r="Q42">
         <v>-0.007050498506968039</v>
       </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
       <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
         <v>0</v>
       </c>
     </row>
@@ -2775,33 +2903,36 @@
         <v>6477293</v>
       </c>
       <c r="I43">
+        <v>92573448185.0683</v>
+      </c>
+      <c r="J43">
         <v>0.00176526656313869</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>8.809848759785607</v>
       </c>
-      <c r="K43">
-        <v>0.461270043895736</v>
-      </c>
       <c r="L43">
-        <v>0.3046957206456042</v>
+        <v>0.2162375221510508</v>
       </c>
       <c r="M43">
-        <v>0.1565743232501318</v>
+        <v>0.1428374734374188</v>
       </c>
       <c r="N43">
-        <v>0.4425957810920735</v>
+        <v>0.07340004871363191</v>
       </c>
       <c r="O43">
-        <v>2.079556966404485</v>
+        <v>0.2074832655716353</v>
       </c>
       <c r="P43">
+        <v>0.9748698220015033</v>
+      </c>
+      <c r="Q43">
         <v>0.001251177006620585</v>
       </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
       <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
         <v>0</v>
       </c>
     </row>
@@ -2819,7 +2950,7 @@
         <v>6010740385.069988</v>
       </c>
       <c r="E44">
-        <v>19500910131.78494</v>
+        <v>19500910131.78493</v>
       </c>
       <c r="F44">
         <v>38052070751.33863</v>
@@ -2831,33 +2962,36 @@
         <v>6502124</v>
       </c>
       <c r="I44">
+        <v>95619926151.52577</v>
+      </c>
+      <c r="J44">
         <v>0.003833545896410717</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>8.830450981670499</v>
       </c>
-      <c r="K44">
-        <v>0.4214793168529491</v>
-      </c>
       <c r="L44">
-        <v>0.2863167008269596</v>
+        <v>0.1960194855692191</v>
       </c>
       <c r="M44">
-        <v>0.1351626160259895</v>
+        <v>0.1331587343954004</v>
       </c>
       <c r="N44">
-        <v>0.4385140364482876</v>
+        <v>0.06286075117381877</v>
       </c>
       <c r="O44">
-        <v>2.035353212429143</v>
+        <v>0.2039419074731608</v>
       </c>
       <c r="P44">
+        <v>0.9465918580085758</v>
+      </c>
+      <c r="Q44">
         <v>0.002338544332217696</v>
       </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
       <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
         <v>0</v>
       </c>
     </row>
@@ -2887,33 +3021,36 @@
         <v>6518946</v>
       </c>
       <c r="I45">
+        <v>100503061534.7117</v>
+      </c>
+      <c r="J45">
         <v>0.002587154597482266</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>8.887028563925851</v>
       </c>
-      <c r="K45">
-        <v>0.5121169602372413</v>
-      </c>
       <c r="L45">
-        <v>0.3379454306223332</v>
+        <v>0.2404112114499246</v>
       </c>
       <c r="M45">
-        <v>0.174171529614908</v>
+        <v>0.1586470995653882</v>
       </c>
       <c r="N45">
-        <v>0.4205766714358639</v>
+        <v>0.08176411188453638</v>
       </c>
       <c r="O45">
-        <v>1.906567522277826</v>
+        <v>0.1974379974461937</v>
       </c>
       <c r="P45">
+        <v>0.8950303218420166</v>
+      </c>
+      <c r="Q45">
         <v>0.006407099974031993</v>
       </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
       <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
         <v>0</v>
       </c>
     </row>
@@ -2943,33 +3080,36 @@
         <v>6552699</v>
       </c>
       <c r="I46">
+        <v>102009215189.7894</v>
+      </c>
+      <c r="J46">
         <v>0.005177677495717958</v>
       </c>
-      <c r="J46">
-        <v>8.857861292276033</v>
-      </c>
       <c r="K46">
-        <v>0.4690838855201794</v>
+        <v>8.857861292276032</v>
       </c>
       <c r="L46">
-        <v>0.3223700047093912</v>
+        <v>0.2118125102526028</v>
       </c>
       <c r="M46">
-        <v>0.1467138808107881</v>
+        <v>0.1455645824454614</v>
       </c>
       <c r="N46">
-        <v>0.4394684223511241</v>
+        <v>0.06624792780714135</v>
       </c>
       <c r="O46">
-        <v>2.108698094655846</v>
+        <v>0.1984397942208532</v>
       </c>
       <c r="P46">
-        <v>-0.003282004940122985</v>
+        <v>0.9521722032694323</v>
       </c>
       <c r="Q46">
-        <v>0</v>
+        <v>-0.003282004940122984</v>
       </c>
       <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
         <v>0</v>
       </c>
     </row>
@@ -2999,33 +3139,36 @@
         <v>6569844</v>
       </c>
       <c r="I47">
+        <v>99849704980.84657</v>
+      </c>
+      <c r="J47">
         <v>0.002616479102732994</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>8.833224501946647</v>
       </c>
-      <c r="K47">
-        <v>0.4617256969786654</v>
-      </c>
       <c r="L47">
-        <v>0.2983444930624281</v>
+        <v>0.2083593411765342</v>
       </c>
       <c r="M47">
-        <v>0.1633812039162373</v>
+        <v>0.1346315841307981</v>
       </c>
       <c r="N47">
-        <v>0.4098410074391023</v>
+        <v>0.07372775704573607</v>
       </c>
       <c r="O47">
-        <v>2.194359541413239</v>
+        <v>0.1849457434488082</v>
       </c>
       <c r="P47">
+        <v>0.9902314541839986</v>
+      </c>
+      <c r="Q47">
         <v>-0.002781347496473963</v>
       </c>
-      <c r="Q47">
-        <v>0</v>
-      </c>
       <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
         <v>0</v>
       </c>
     </row>
@@ -3055,33 +3198,36 @@
         <v>6586843</v>
       </c>
       <c r="I48">
+        <v>101524308362.8388</v>
+      </c>
+      <c r="J48">
         <v>0.00258742825552627</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>8.84976426269793</v>
       </c>
-      <c r="K48">
-        <v>0.4709359408806262</v>
-      </c>
       <c r="L48">
-        <v>0.3104510579581129</v>
+        <v>0.2130457593659216</v>
       </c>
       <c r="M48">
-        <v>0.1604848829225133</v>
+        <v>0.1404443272368657</v>
       </c>
       <c r="N48">
-        <v>0.4228518511516398</v>
+        <v>0.07260143212905593</v>
       </c>
       <c r="O48">
-        <v>2.150508826572588</v>
+        <v>0.1912930951063727</v>
       </c>
       <c r="P48">
+        <v>0.9728643456762808</v>
+      </c>
+      <c r="Q48">
         <v>0.001872448814998151</v>
       </c>
-      <c r="Q48">
-        <v>0</v>
-      </c>
       <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
         <v>0</v>
       </c>
     </row>
@@ -3105,39 +3251,42 @@
         <v>40607252775.8662</v>
       </c>
       <c r="G49">
-        <v>63903294632.2572</v>
+        <v>63903294632.25719</v>
       </c>
       <c r="H49">
         <v>6603335</v>
       </c>
       <c r="I49">
+        <v>110895828846.8262</v>
+      </c>
+      <c r="J49">
         <v>0.002503779124536587</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>8.913735498794038</v>
       </c>
-      <c r="K49">
-        <v>0.582666210388506</v>
-      </c>
       <c r="L49">
-        <v>0.3493749273291671</v>
+        <v>0.2579016335483535</v>
       </c>
       <c r="M49">
-        <v>0.2332912830593388</v>
+        <v>0.1546414788991289</v>
       </c>
       <c r="N49">
-        <v>0.4032754691215863</v>
+        <v>0.1032601546492247</v>
       </c>
       <c r="O49">
-        <v>2.129171536785418</v>
+        <v>0.1784991139044904</v>
       </c>
       <c r="P49">
+        <v>0.9424209052305975</v>
+      </c>
+      <c r="Q49">
         <v>0.007228580807033369</v>
       </c>
-      <c r="Q49">
-        <v>0</v>
-      </c>
       <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
         <v>0</v>
       </c>
     </row>
@@ -3167,33 +3316,36 @@
         <v>6638252</v>
       </c>
       <c r="I50">
+        <v>107193557665.6671</v>
+      </c>
+      <c r="J50">
         <v>0.005287782612876768</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>8.870486691530923</v>
       </c>
-      <c r="K50">
-        <v>0.4753754431675812</v>
-      </c>
       <c r="L50">
-        <v>0.3141905937342203</v>
+        <v>0.2095681189089555</v>
       </c>
       <c r="M50">
-        <v>0.1611848494333609</v>
+        <v>0.138510166341421</v>
       </c>
       <c r="N50">
-        <v>0.3978662632560891</v>
+        <v>0.07105795256753449</v>
       </c>
       <c r="O50">
-        <v>2.264841422216497</v>
+        <v>0.1753983836698111</v>
       </c>
       <c r="P50">
+        <v>0.9984498848285551</v>
+      </c>
+      <c r="Q50">
         <v>-0.004851928494957747</v>
       </c>
-      <c r="Q50">
-        <v>0</v>
-      </c>
       <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
         <v>1</v>
       </c>
     </row>
@@ -3223,33 +3375,36 @@
         <v>6659818.799678822</v>
       </c>
       <c r="I51">
+        <v>98340557380.74973</v>
+      </c>
+      <c r="J51">
         <v>0.003248867273918155</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>8.767916834364783</v>
       </c>
-      <c r="K51">
-        <v>0.4498891937262053</v>
-      </c>
       <c r="L51">
-        <v>0.3266999287165317</v>
+        <v>0.1957461406027551</v>
       </c>
       <c r="M51">
-        <v>0.1231892650096736</v>
+        <v>0.1421466687203322</v>
       </c>
       <c r="N51">
-        <v>0.4033673870513345</v>
+        <v>0.05359947188242285</v>
       </c>
       <c r="O51">
-        <v>2.257203846809817</v>
+        <v>0.1755045694837664</v>
       </c>
       <c r="P51">
+        <v>0.9821061446423839</v>
+      </c>
+      <c r="Q51">
         <v>-0.0115630472975139</v>
       </c>
-      <c r="Q51">
-        <v>0</v>
-      </c>
       <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
         <v>1</v>
       </c>
     </row>
@@ -3279,33 +3434,36 @@
         <v>6682508.564685112</v>
       </c>
       <c r="I52">
+        <v>100714633471.8687</v>
+      </c>
+      <c r="J52">
         <v>0.003406964316714445</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>8.790504709023759</v>
       </c>
-      <c r="K52">
-        <v>0.5099648836562928</v>
-      </c>
       <c r="L52">
-        <v>0.3370151302245329</v>
+        <v>0.2223590998338309</v>
       </c>
       <c r="M52">
-        <v>0.1729497534317599</v>
+        <v>0.1469481201329454</v>
       </c>
       <c r="N52">
-        <v>0.3265251349910023</v>
+        <v>0.07541097970088548</v>
       </c>
       <c r="O52">
-        <v>2.090278253520488</v>
+        <v>0.1423741857854166</v>
       </c>
       <c r="P52">
+        <v>0.9114203855030725</v>
+      </c>
+      <c r="Q52">
         <v>0.002576196271666831</v>
       </c>
-      <c r="Q52">
-        <v>0</v>
-      </c>
       <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
         <v>1</v>
       </c>
     </row>
@@ -3335,33 +3493,36 @@
         <v>6706644.772098123</v>
       </c>
       <c r="I53">
+        <v>104738841786.9918</v>
+      </c>
+      <c r="J53">
         <v>0.003611848332011489</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>8.831448025477314</v>
       </c>
-      <c r="K53">
-        <v>0.6088178608871343</v>
-      </c>
       <c r="L53">
-        <v>0.3748425664146136</v>
+        <v>0.2668910844105784</v>
       </c>
       <c r="M53">
-        <v>0.2339752944725207</v>
+        <v>0.1643219515404243</v>
       </c>
       <c r="N53">
-        <v>0.2259380532336192</v>
+        <v>0.1025691328701541</v>
       </c>
       <c r="O53">
-        <v>1.978961526072515</v>
+        <v>0.09904579991997724</v>
       </c>
       <c r="P53">
+        <v>0.8675290618621008</v>
+      </c>
+      <c r="Q53">
         <v>0.004657675276770634</v>
       </c>
-      <c r="Q53">
-        <v>0</v>
-      </c>
       <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
         <v>1</v>
       </c>
     </row>
@@ -3391,33 +3552,36 @@
         <v>6732726.012470978</v>
       </c>
       <c r="I54">
+        <v>101139169199.1667</v>
+      </c>
+      <c r="J54">
         <v>0.003888865633880214</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>8.759440905663116</v>
       </c>
-      <c r="K54">
-        <v>0.4599106781368548</v>
-      </c>
       <c r="L54">
-        <v>0.3212057703861472</v>
+        <v>0.1950391979703996</v>
       </c>
       <c r="M54">
-        <v>0.1387049077507076</v>
+        <v>0.1362171369740116</v>
       </c>
       <c r="N54">
-        <v>0.2241914422287416</v>
+        <v>0.05882206099638809</v>
       </c>
       <c r="O54">
-        <v>2.213434179457687</v>
+        <v>0.09507524213453779</v>
       </c>
       <c r="P54">
-        <v>-0.008153489621007704</v>
+        <v>0.9386745027764606</v>
       </c>
       <c r="Q54">
-        <v>0</v>
+        <v>-0.008153489621007703</v>
       </c>
       <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
         <v>1</v>
       </c>
     </row>
@@ -3447,33 +3611,36 @@
         <v>6756554.048099764</v>
       </c>
       <c r="I55">
-        <v>0.003539136389131076</v>
+        <v>101726645661.7535</v>
       </c>
       <c r="J55">
+        <v>0.003539136389131075</v>
+      </c>
+      <c r="K55">
         <v>8.730613727513049</v>
       </c>
-      <c r="K55">
-        <v>0.5190887673735403</v>
-      </c>
       <c r="L55">
-        <v>0.3595184342395085</v>
+        <v>0.2133975984485832</v>
       </c>
       <c r="M55">
-        <v>0.1595703331340318</v>
+        <v>0.1477981711160731</v>
       </c>
       <c r="N55">
-        <v>0.2307861788674422</v>
+        <v>0.06559942733251004</v>
       </c>
       <c r="O55">
-        <v>2.359578278027843</v>
+        <v>0.09487628980034779</v>
       </c>
       <c r="P55">
+        <v>0.9700235673183852</v>
+      </c>
+      <c r="Q55">
         <v>-0.00329098380370707</v>
       </c>
-      <c r="Q55">
-        <v>0</v>
-      </c>
       <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
         <v>1</v>
       </c>
     </row>
@@ -3503,33 +3670,36 @@
         <v>6780956.719137883</v>
       </c>
       <c r="I56">
+        <v>104528159885.5606</v>
+      </c>
+      <c r="J56">
         <v>0.003611703667934306</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>8.760069743678756</v>
       </c>
-      <c r="K56">
-        <v>0.4528551088034856</v>
-      </c>
       <c r="L56">
-        <v>0.3337922991426811</v>
+        <v>0.1872694304099843</v>
       </c>
       <c r="M56">
-        <v>0.1190628096608045</v>
+        <v>0.1380333190915033</v>
       </c>
       <c r="N56">
-        <v>0.250877202422951</v>
+        <v>0.04923611131848098</v>
       </c>
       <c r="O56">
-        <v>2.321089999591938</v>
+        <v>0.10374539204102</v>
       </c>
       <c r="P56">
+        <v>0.9598416661398769</v>
+      </c>
+      <c r="Q56">
         <v>0.003373876921490826</v>
       </c>
-      <c r="Q56">
-        <v>0</v>
-      </c>
       <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
         <v>1</v>
       </c>
     </row>
@@ -3559,33 +3729,36 @@
         <v>6805794.607562329</v>
       </c>
       <c r="I57">
+        <v>113219847142.0416</v>
+      </c>
+      <c r="J57">
         <v>0.003662888505739271</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>8.834280776562661</v>
       </c>
-      <c r="K57">
-        <v>0.6991071983630351</v>
-      </c>
       <c r="L57">
-        <v>0.4440379835744523</v>
+        <v>0.2885223367313002</v>
       </c>
       <c r="M57">
-        <v>0.2550692147885829</v>
+        <v>0.1832549813795905</v>
       </c>
       <c r="N57">
-        <v>0.2016497730760078</v>
+        <v>0.1052673553517097</v>
       </c>
       <c r="O57">
-        <v>2.17459572341662</v>
+        <v>0.08322109093634882</v>
       </c>
       <c r="P57">
+        <v>0.897458130934945</v>
+      </c>
+      <c r="Q57">
         <v>0.00847151164948845</v>
       </c>
-      <c r="Q57">
-        <v>0</v>
-      </c>
       <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
         <v>1</v>
       </c>
     </row>
@@ -3609,39 +3782,42 @@
         <v>53053545621.79591</v>
       </c>
       <c r="G58">
-        <v>53581884864.71298</v>
+        <v>53581884864.71297</v>
       </c>
       <c r="H58">
         <v>6830810.316637572</v>
       </c>
       <c r="I58">
+        <v>109989996205.692</v>
+      </c>
+      <c r="J58">
         <v>0.003675648549171216</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>8.769004983324853</v>
       </c>
-      <c r="K58">
-        <v>0.5254118692224336</v>
-      </c>
       <c r="L58">
-        <v>0.3659539774139257</v>
+        <v>0.2098695319966576</v>
       </c>
       <c r="M58">
-        <v>0.1594578918085078</v>
+        <v>0.1461759706453483</v>
       </c>
       <c r="N58">
-        <v>0.260793987231179</v>
+        <v>0.06369356135130937</v>
       </c>
       <c r="O58">
-        <v>2.427162339261106</v>
+        <v>0.1041710613213778</v>
       </c>
       <c r="P58">
+        <v>0.9695011743348938</v>
+      </c>
+      <c r="Q58">
         <v>-0.007388919923281612</v>
       </c>
-      <c r="Q58">
-        <v>0</v>
-      </c>
       <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="S58">
         <v>1</v>
       </c>
     </row>
@@ -3656,7 +3832,7 @@
         <v>16895447044.36875</v>
       </c>
       <c r="D59">
-        <v>7863200173.391769</v>
+        <v>7863200173.391768</v>
       </c>
       <c r="E59">
         <v>8654193126.555441</v>
@@ -3671,33 +3847,36 @@
         <v>6855553.863302106</v>
       </c>
       <c r="I59">
+        <v>99491314405.30119</v>
+      </c>
+      <c r="J59">
         <v>0.003622344277993968</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>8.647739919354713</v>
       </c>
-      <c r="K59">
-        <v>0.6338969123560931</v>
-      </c>
       <c r="L59">
-        <v>0.4325749957218372</v>
+        <v>0.248852348225096</v>
       </c>
       <c r="M59">
-        <v>0.201321916634256</v>
+        <v>0.1698183117326321</v>
       </c>
       <c r="N59">
-        <v>0.2215737497128499</v>
+        <v>0.07903403649246385</v>
       </c>
       <c r="O59">
-        <v>2.102301807276993</v>
+        <v>0.08698440842082512</v>
       </c>
       <c r="P59">
+        <v>0.8253120203318718</v>
+      </c>
+      <c r="Q59">
         <v>-0.01382882826509257</v>
       </c>
-      <c r="Q59">
-        <v>0</v>
-      </c>
       <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
         <v>1</v>
       </c>
     </row>
@@ -3727,33 +3906,36 @@
         <v>6880529.648652307</v>
       </c>
       <c r="I60">
+        <v>108728566883.9486</v>
+      </c>
+      <c r="J60">
         <v>0.003643146250209691</v>
       </c>
-      <c r="J60">
-        <v>8.735640413632194</v>
-      </c>
       <c r="K60">
-        <v>0.48911257628562</v>
+        <v>8.735640413632193</v>
       </c>
       <c r="L60">
-        <v>0.3202541801682902</v>
+        <v>0.1925428802293085</v>
       </c>
       <c r="M60">
-        <v>0.1688583961173298</v>
+        <v>0.1260704901995205</v>
       </c>
       <c r="N60">
-        <v>0.2453094512249399</v>
+        <v>0.06647239002978798</v>
       </c>
       <c r="O60">
-        <v>2.2496653193276</v>
+        <v>0.0965679284818456</v>
       </c>
       <c r="P60">
+        <v>0.8855978380780352</v>
+      </c>
+      <c r="Q60">
         <v>0.01016456265997867</v>
       </c>
-      <c r="Q60">
-        <v>0</v>
-      </c>
       <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
         <v>1</v>
       </c>
     </row>
@@ -3783,33 +3965,36 @@
         <v>6905650.509846144</v>
       </c>
       <c r="I61">
-        <v>0.003651006895778537</v>
+        <v>117185446014.0772</v>
       </c>
       <c r="J61">
+        <v>0.003651006895778536</v>
+      </c>
+      <c r="K61">
         <v>8.79934407255694</v>
       </c>
-      <c r="K61">
-        <v>0.7393360793270596</v>
-      </c>
       <c r="L61">
-        <v>0.4243875455316106</v>
+        <v>0.2888546698794033</v>
       </c>
       <c r="M61">
-        <v>0.314948533795449</v>
+        <v>0.1658059545491695</v>
       </c>
       <c r="N61">
-        <v>0.2638713542814507</v>
+        <v>0.1230487153302338</v>
       </c>
       <c r="O61">
-        <v>2.231366203442386</v>
+        <v>0.103093133235125</v>
       </c>
       <c r="P61">
+        <v>0.8717828956244984</v>
+      </c>
+      <c r="Q61">
         <v>0.007292385664745771</v>
       </c>
-      <c r="Q61">
-        <v>0</v>
-      </c>
       <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
         <v>1</v>
       </c>
     </row>
@@ -3839,33 +4024,36 @@
         <v>6930842.574915958</v>
       </c>
       <c r="I62">
+        <v>118293589725.8603</v>
+      </c>
+      <c r="J62">
         <v>0.003648036493288352</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>8.79108379318315</v>
       </c>
-      <c r="K62">
-        <v>0.649483234854967</v>
-      </c>
       <c r="L62">
-        <v>0.4228970028683795</v>
+        <v>0.2502141982847392</v>
       </c>
       <c r="M62">
-        <v>0.2265862319865875</v>
+        <v>0.1629215795745053</v>
       </c>
       <c r="N62">
-        <v>0.3008300056466655</v>
+        <v>0.0872926187102339</v>
       </c>
       <c r="O62">
-        <v>2.569415677789493</v>
+        <v>0.1158951219113186</v>
       </c>
       <c r="P62">
+        <v>0.9898704837576013</v>
+      </c>
+      <c r="Q62">
         <v>-0.0009387380815749635</v>
       </c>
-      <c r="Q62">
-        <v>0</v>
-      </c>
       <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
         <v>1</v>
       </c>
     </row>
@@ -3895,33 +4083,36 @@
         <v>6956078.697855364</v>
       </c>
       <c r="I63">
+        <v>119916245236.831</v>
+      </c>
+      <c r="J63">
         <v>0.003641133479317637</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>8.799282727611473</v>
       </c>
-      <c r="K63">
-        <v>0.5413187366412734</v>
-      </c>
       <c r="L63">
-        <v>0.3413635901770553</v>
+        <v>0.2081706307067226</v>
       </c>
       <c r="M63">
-        <v>0.1999551464642182</v>
+        <v>0.131275474239793</v>
       </c>
       <c r="N63">
-        <v>0.391454269359703</v>
+        <v>0.07689515646692964</v>
       </c>
       <c r="O63">
-        <v>2.932612188465644</v>
+        <v>0.1505384473684878</v>
       </c>
       <c r="P63">
+        <v>1.127771288093575</v>
+      </c>
+      <c r="Q63">
         <v>0.0009326420520165968</v>
       </c>
-      <c r="Q63">
-        <v>0</v>
-      </c>
       <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
         <v>1</v>
       </c>
     </row>
@@ -3951,33 +4142,36 @@
         <v>6981439.383677662</v>
       </c>
       <c r="I64">
+        <v>122605681355.0494</v>
+      </c>
+      <c r="J64">
         <v>0.003645830779648554</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>8.818352164336442</v>
       </c>
-      <c r="K64">
-        <v>0.6532179642097604</v>
-      </c>
       <c r="L64">
-        <v>0.3686888936154639</v>
+        <v>0.2513357000293618</v>
       </c>
       <c r="M64">
-        <v>0.2845290705942964</v>
+        <v>0.1418587458506227</v>
       </c>
       <c r="N64">
-        <v>0.3480628689792576</v>
+        <v>0.1094769541787392</v>
       </c>
       <c r="O64">
-        <v>2.948211832960756</v>
+        <v>0.1339225643234731</v>
       </c>
       <c r="P64">
+        <v>1.134370034921596</v>
+      </c>
+      <c r="Q64">
         <v>0.002167158087230225</v>
       </c>
-      <c r="Q64">
-        <v>0</v>
-      </c>
       <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
         <v>1</v>
       </c>
     </row>
@@ -4004,36 +4198,39 @@
         <v>80204272320.48616</v>
       </c>
       <c r="H65">
-        <v>7006897.215738813</v>
+        <v>7006897.215738812</v>
       </c>
       <c r="I65">
+        <v>136708254887.9271</v>
+      </c>
+      <c r="J65">
         <v>0.00364650191200827</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>8.882213840046701</v>
       </c>
-      <c r="K65">
-        <v>0.8451586131232545</v>
-      </c>
       <c r="L65">
-        <v>0.4790109254240944</v>
+        <v>0.3120079693686669</v>
       </c>
       <c r="M65">
-        <v>0.3661476876991602</v>
+        <v>0.1768368964432262</v>
       </c>
       <c r="N65">
-        <v>0.3176923090160375</v>
+        <v>0.1351710729254407</v>
       </c>
       <c r="O65">
-        <v>2.761180595409062</v>
+        <v>0.1172827569653855</v>
       </c>
       <c r="P65">
+        <v>1.019347536967134</v>
+      </c>
+      <c r="Q65">
         <v>0.007241905802824578</v>
       </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
       <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
         <v>1</v>
       </c>
     </row>
@@ -4057,39 +4254,42 @@
         <v>69422835331.33748</v>
       </c>
       <c r="G66">
-        <v>87094636791.04775</v>
+        <v>87094636791.04774</v>
       </c>
       <c r="H66">
         <v>7032439.988343691</v>
       </c>
       <c r="I66">
+        <v>132477595344.6158</v>
+      </c>
+      <c r="J66">
         <v>0.003645375666065704</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>8.82327272379948</v>
       </c>
-      <c r="K66">
-        <v>0.6404953544631538</v>
-      </c>
       <c r="L66">
-        <v>0.4195958034684312</v>
+        <v>0.2308757071954489</v>
       </c>
       <c r="M66">
-        <v>0.2208995509947225</v>
+        <v>0.1512493060050596</v>
       </c>
       <c r="N66">
-        <v>0.3625761162689962</v>
+        <v>0.07962640119038931</v>
       </c>
       <c r="O66">
-        <v>3.277616475762642</v>
+        <v>0.1306957445865432</v>
       </c>
       <c r="P66">
+        <v>1.181463716300361</v>
+      </c>
+      <c r="Q66">
         <v>-0.006635858729439281</v>
       </c>
-      <c r="Q66">
-        <v>0</v>
-      </c>
       <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
         <v>1</v>
       </c>
     </row>
@@ -4104,7 +4304,7 @@
         <v>18103399256.1731</v>
       </c>
       <c r="D67">
-        <v>12207388525.45355</v>
+        <v>12207388525.45354</v>
       </c>
       <c r="E67">
         <v>17633591222.05977</v>
@@ -4119,33 +4319,36 @@
         <v>7058071.195923326</v>
       </c>
       <c r="I67">
+        <v>137350772260.7607</v>
+      </c>
+      <c r="J67">
         <v>0.003644710459260041</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>8.829409300659984</v>
       </c>
-      <c r="K67">
-        <v>0.6285610292780781</v>
-      </c>
       <c r="L67">
-        <v>0.3754139071499082</v>
+        <v>0.2206815970723597</v>
       </c>
       <c r="M67">
-        <v>0.2531471221281699</v>
+        <v>0.1318041315545264</v>
       </c>
       <c r="N67">
-        <v>0.3656714014911016</v>
+        <v>0.08887746551783335</v>
       </c>
       <c r="O67">
-        <v>3.482393039854217</v>
+        <v>0.1283836336106094</v>
       </c>
       <c r="P67">
+        <v>1.22263395576933</v>
+      </c>
+      <c r="Q67">
         <v>0.0006954989438274772</v>
       </c>
-      <c r="Q67">
-        <v>0</v>
-      </c>
       <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
         <v>1</v>
       </c>
     </row>
@@ -4175,33 +4378,36 @@
         <v>7083802.133478085</v>
       </c>
       <c r="I68">
+        <v>139926753974.2322</v>
+      </c>
+      <c r="J68">
         <v>0.003645604704245642</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>8.836906354226324</v>
       </c>
-      <c r="K68">
-        <v>0.6126839515072634</v>
-      </c>
       <c r="L68">
-        <v>0.3665469799352956</v>
+        <v>0.2135117763777452</v>
       </c>
       <c r="M68">
-        <v>0.2461369715719678</v>
+        <v>0.1277364889668648</v>
       </c>
       <c r="N68">
-        <v>0.3745259400353874</v>
+        <v>0.08577528741088036</v>
       </c>
       <c r="O68">
-        <v>3.377131455200565</v>
+        <v>0.1305170448153193</v>
       </c>
       <c r="P68">
+        <v>1.176883014949485</v>
+      </c>
+      <c r="Q68">
         <v>0.0008491002411428195</v>
       </c>
-      <c r="Q68">
-        <v>0</v>
-      </c>
       <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
         <v>1</v>
       </c>
     </row>
@@ -4231,33 +4437,36 @@
         <v>7109626.475491483</v>
       </c>
       <c r="I69">
+        <v>152453306934.7087</v>
+      </c>
+      <c r="J69">
         <v>0.003645548185394914</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>8.891648125517181</v>
       </c>
-      <c r="K69">
-        <v>0.7026324406895242</v>
-      </c>
       <c r="L69">
-        <v>0.414585573485412</v>
+        <v>0.2382494180334141</v>
       </c>
       <c r="M69">
-        <v>0.2880468672041123</v>
+        <v>0.1405781542210272</v>
       </c>
       <c r="N69">
-        <v>0.342869219606984</v>
+        <v>0.09767126381238699</v>
       </c>
       <c r="O69">
-        <v>3.064702574590342</v>
+        <v>0.1162604902682409</v>
       </c>
       <c r="P69">
+        <v>1.039182882198142</v>
+      </c>
+      <c r="Q69">
         <v>0.006194675952934103</v>
       </c>
-      <c r="Q69">
-        <v>0</v>
-      </c>
       <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
         <v>1</v>
       </c>
     </row>

</xml_diff>